<commit_message>
Unit tests on Linear Programming
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/LinearProgTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/LinearProgTest.xlsx
@@ -1,63 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\jacobi\src\test\resources\jacobi\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="22995" windowHeight="7485"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="22995" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="4x7" sheetId="1" r:id="rId1"/>
+    <sheet name="3x8" sheetId="2" r:id="rId2"/>
     <sheet name="rand" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$A$29:$G$29</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'3x8'!$A$28:$H$28</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'4x7'!$A$29:$G$29</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$A$32</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$A$33</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$A$34</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$A$35</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'3x8'!$A$31</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'4x7'!$A$32</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'3x8'!$A$32</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'4x7'!$A$33</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'3x8'!$A$33</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'4x7'!$A$34</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'4x7'!$A$35</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$A$26</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'3x8'!$A$25</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'4x7'!$A$26</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$A$20</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$A$21</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$A$22</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$A$23</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'3x8'!$A$20</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'4x7'!$A$20</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'3x8'!$A$21</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'4x7'!$A$21</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'3x8'!$A$22</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'4x7'!$A$22</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'4x7'!$A$23</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>#0</t>
   </si>
@@ -77,7 +118,19 @@
     <t>Constraint</t>
   </si>
   <si>
-    <t>Answer=</t>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>Target=</t>
+  </si>
+  <si>
+    <t>Variables=</t>
+  </si>
+  <si>
+    <t>Constraints=</t>
   </si>
 </sst>
 </file>
@@ -124,6 +177,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -172,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,37 +495,37 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>19.033179172810648</v>
+        <v>10.519907092277197</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20.367922772176215</v>
+        <v>24.69602143585513</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.88914781993704395</v>
+        <v>0.32961454104736987</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5.8736313099516337</v>
+        <v>-11.473286835905338</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>18.371585311848847</v>
+        <v>0.19063820971791401</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>22.691739816890575</v>
+        <v>10.690781058751099</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-15.243601419106167</v>
+        <v>4.9725552511727571</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -487,94 +543,94 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11.687811499068125</v>
+        <v>14.445953148932269</v>
       </c>
       <c r="B13">
-        <v>-10.248592397900696</v>
+        <v>26.111918916047919</v>
       </c>
       <c r="C13">
-        <v>3.8778398766759032</v>
+        <v>13.847207533091044</v>
       </c>
       <c r="D13">
-        <v>2.0686939540137175</v>
+        <v>13.482686464783505</v>
       </c>
       <c r="E13">
-        <v>-18.007448061008816</v>
+        <v>24.333640677413214</v>
       </c>
       <c r="F13">
-        <v>23.237642809234842</v>
+        <v>2.6729336796036947</v>
       </c>
       <c r="G13">
-        <v>28.504945690946393</v>
+        <v>29.38514286384072</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>20.791375365725877</v>
+        <v>-15.758094557866341</v>
       </c>
       <c r="B14">
-        <v>25.827194525085602</v>
+        <v>1.9363753066345524</v>
       </c>
       <c r="C14">
-        <v>-0.52235366034765107</v>
+        <v>-5.6929339104128438</v>
       </c>
       <c r="D14">
-        <v>12.672208694551969</v>
+        <v>3.9915279056864676</v>
       </c>
       <c r="E14">
-        <v>-18.309995109472638</v>
+        <v>12.700886717777067</v>
       </c>
       <c r="F14">
-        <v>-2.2502154359372071</v>
+        <v>15.180563850014707</v>
       </c>
       <c r="G14">
-        <v>12.692128225888709</v>
+        <v>18.842313632947992</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-4.1493867334473347</v>
+        <v>19.335503183010587</v>
       </c>
       <c r="B15">
-        <v>-10.235944015327446</v>
+        <v>10.876338028412565</v>
       </c>
       <c r="C15">
-        <v>9.7384674293461764</v>
+        <v>-8.6302913434516011</v>
       </c>
       <c r="D15">
-        <v>11.403583739416383</v>
+        <v>24.024786754155613</v>
       </c>
       <c r="E15">
-        <v>-16.931987398880764</v>
+        <v>-0.91379446339794868</v>
       </c>
       <c r="F15">
-        <v>14.331991754703012</v>
+        <v>-19.42413559646829</v>
       </c>
       <c r="G15">
-        <v>1.01349201985715</v>
+        <v>-4.1546963226139422</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-11.467682640200149</v>
+        <v>-15.462653384327439</v>
       </c>
       <c r="B16">
-        <v>6.0143958393058412</v>
+        <v>4.6370859212902182</v>
       </c>
       <c r="C16">
-        <v>-1.0618710764013883</v>
+        <v>23.106512057175493</v>
       </c>
       <c r="D16">
-        <v>13.775875864920138</v>
+        <v>7.4973674955735952</v>
       </c>
       <c r="E16">
-        <v>3.9988666052189039</v>
+        <v>24.901354988866181</v>
       </c>
       <c r="F16">
-        <v>-17.043475875253161</v>
+        <v>8.8183231377610269</v>
       </c>
       <c r="G16">
-        <v>-2.3916314121211677</v>
+        <v>-7.6117586419132017</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -592,22 +648,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>25.341587474298692</v>
+        <v>5.2544854091102486</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>13.947687994706385</v>
+        <v>6.1454857586866538</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>19.387311838429504</v>
+        <v>17.553572864360554</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.9542161393475439</v>
+        <v>13.817652344719328</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,7 +674,7 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="array" ref="A26">MMULT(A29:G29,A3:A9)</f>
-        <v>24.746258225693669</v>
+        <v>9.5656365401299936</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -628,7 +684,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>0.24229227468981646</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -643,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1.0905403651452859</v>
+        <v>0.65633598543045257</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -657,30 +713,93 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>SUMPRODUCT(A$29:G$29,A13:G13)</f>
-        <v>25.341587474298692</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5.2544854091102531</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ref="A33:A35" si="0">SUMPRODUCT(A$29:G$29,A14:G14)</f>
-        <v>-2.4539507631625206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6.1454857586866538</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>15.629615521433049</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>-8.0639161293589261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>-18.586598404343452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2.0413013452376605</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="array" ref="A39:A45">TRANSPOSE(A29:G29)</f>
+        <v>0.24229227468981646</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.65633598543045257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f>A26</f>
+        <v>9.5656365401299936</v>
       </c>
     </row>
   </sheetData>
@@ -690,12 +809,323 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25.736754976807042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>18.574186919974075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>17.798060619724673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22.358990664213955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-18.224376839054873</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5.3233710763485718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>13.719897130214719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>25.085104018476734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.833273927718853</v>
+      </c>
+      <c r="B14">
+        <v>24.058863245705716</v>
+      </c>
+      <c r="C14">
+        <v>-17.193417171918732</v>
+      </c>
+      <c r="D14">
+        <v>21.130207257469614</v>
+      </c>
+      <c r="E14">
+        <v>-5.5453936540250819</v>
+      </c>
+      <c r="F14">
+        <v>26.845107184779309</v>
+      </c>
+      <c r="G14">
+        <v>6.0232456497256344</v>
+      </c>
+      <c r="H14">
+        <v>-11.908798726002876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.6459143369696179</v>
+      </c>
+      <c r="B15">
+        <v>-13.799037376571814</v>
+      </c>
+      <c r="C15">
+        <v>9.9949976327992545</v>
+      </c>
+      <c r="D15">
+        <v>10.316340508652289</v>
+      </c>
+      <c r="E15">
+        <v>1.5550244897739347</v>
+      </c>
+      <c r="F15">
+        <v>-15.67355317625657</v>
+      </c>
+      <c r="G15">
+        <v>26.296925581161602</v>
+      </c>
+      <c r="H15">
+        <v>8.2627516374041647</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-4.542950683388673</v>
+      </c>
+      <c r="B16">
+        <v>26.054988517421314</v>
+      </c>
+      <c r="C16">
+        <v>2.7866100816797861</v>
+      </c>
+      <c r="D16">
+        <v>-14.341535693703099</v>
+      </c>
+      <c r="E16">
+        <v>8.2940859594922252</v>
+      </c>
+      <c r="F16">
+        <v>29.675080402067643</v>
+      </c>
+      <c r="G16">
+        <v>18.323312800613877</v>
+      </c>
+      <c r="H16">
+        <v>-5.8671161450215052</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-3.1241180677875739</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8.9442811308992702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11.651455956436141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="array" ref="A25">MMULT(A28:H28,A3:A10)</f>
+        <v>96.448607024871933</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1.1661703755674175</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.13620068337387189</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>2.8599694315673352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="array" ref="A31:A33">MMULT(A14:H16,TRANSPOSE(A28:H28))</f>
+        <v>-3.1241180677875704</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8.9442811308992702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11.651455956436138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="array" ref="A37:A44">TRANSPOSE(A28:H28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.1661703755674175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.13620068337387189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2.8599694315673352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>A25</f>
+        <v>96.448607024871933</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -704,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,1381 +1143,1381 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*50-20</f>
-        <v>27.915150241637861</v>
+        <v>22.049957430548027</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:K16" ca="1" si="0">RAND()*50-20</f>
-        <v>-15.925041491518487</v>
+        <v>6.4244930061626064</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.299214335588825</v>
+        <v>-0.19488996941212022</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0830447591808827</v>
+        <v>10.447759656590673</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0717003717801106</v>
+        <v>-15.495220006715027</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>20.585771377741374</v>
+        <v>29.858095585918214</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.509229689475564</v>
+        <v>12.393187184230669</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>28.930067142365026</v>
+        <v>17.326573748026767</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.1769589453850049</v>
+        <v>-10.523063176592844</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1131936137858141</v>
+        <v>-4.2406495615333419</v>
       </c>
       <c r="K1">
         <f t="shared" ca="1" si="0"/>
-        <v>14.308204970587347</v>
+        <v>17.669375381266754</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:K30" ca="1" si="1">RAND()*50-20</f>
-        <v>19.95176855337462</v>
+        <v>6.3596907791419319</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.884334281264316</v>
+        <v>27.751095846873667</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>23.891821999013295</v>
+        <v>10.722652245318432</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>14.757434225992895</v>
+        <v>0.81677974440653145</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.71243279615917</v>
+        <v>3.50142887504893</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.139942393245633</v>
+        <v>15.087944463176989</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3062907002402717</v>
+        <v>17.974727677408119</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>19.903929844706084</v>
+        <v>21.107329225014638</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78166331601045869</v>
+        <v>-12.937459810869665</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.061105723144131</v>
+        <v>24.033214320050476</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>15.017285430849327</v>
+        <v>7.7104199139980416</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6857842625099941</v>
+        <v>-16.372049067787295</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>24.587471828831035</v>
+        <v>-13.251412971356851</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8987892522831249</v>
+        <v>-14.021899030945738</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.9718837191806671</v>
+        <v>4.4431192442420944</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.2824656886445354</v>
+        <v>27.833471743020247</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.9950888148026742</v>
+        <v>14.178886553866015</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5303001287337281</v>
+        <v>-10.578160090469629</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.681980663529517</v>
+        <v>5.1856093108833505</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.80808199110604</v>
+        <v>-10.57968705989733</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.04166315190702</v>
+        <v>-12.539841782007853</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>26.497064595469212</v>
+        <v>6.4224453075309711</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.16125761666086</v>
+        <v>0.84920957481224235</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>16.074079548684097</v>
+        <v>11.106733062938385</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>22.220192384525809</v>
+        <v>23.457893550316392</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>21.535578661656565</v>
+        <v>13.16965415170759</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>25.131294969641566</v>
+        <v>8.3335983078360449</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.6994706901430678</v>
+        <v>21.679660242134354</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.9491774042616807</v>
+        <v>13.62953361041604</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.89660351290593</v>
+        <v>-6.9484527508860801</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>8.5603240024746086</v>
+        <v>5.2055897876421859</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5042174192032292</v>
+        <v>19.303064032101261</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.762782169031059</v>
+        <v>-18.735947593258555</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.3010837110227698</v>
+        <v>4.8151627762259466</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.942408629504463</v>
+        <v>14.491710963537166</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>16.459590179183728</v>
+        <v>24.981205352417724</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>13.242375723458565</v>
+        <v>-3.9317817444896299</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2409337960977496</v>
+        <v>14.674608856904435</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>20.676940927205905</v>
+        <v>-1.5121849446802003</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1662340264671407</v>
+        <v>-5.7537953284495451</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>18.26060551067706</v>
+        <v>-11.13866953751511</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>17.111847097546473</v>
+        <v>-15.297602748374777</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4656521923581529</v>
+        <v>-3.2011388225583133</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4675169666592076</v>
+        <v>-12.059039677469789</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>13.567985433335004</v>
+        <v>19.932283733579148</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.159102178845458</v>
+        <v>-10.20289190688327</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.260341854168857</v>
+        <v>28.82939476763903</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.468899196037611</v>
+        <v>6.828042375516592</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>27.902298772320421</v>
+        <v>23.021411507286253</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.967554076199125</v>
+        <v>10.763178470648267</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>14.698900950900828</v>
+        <v>0.91703944163296569</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>17.025544824340962</v>
+        <v>-0.39726352592972347</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.916764241578063</v>
+        <v>19.413758873338558</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4957176472909239</v>
+        <v>13.201080469729924</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.9455347248348467</v>
+        <v>10.877497774874175</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>14.959670525010651</v>
+        <v>-19.282406479969659</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>27.613711928773832</v>
+        <v>2.6371358388436192</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>25.587022720434277</v>
+        <v>0.51857109850869776</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.642617474675188</v>
+        <v>5.095941018429464</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>25.366034814774743</v>
+        <v>17.977789277777958</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>20.262092948243044</v>
+        <v>20.042795297040733</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>26.493278822556803</v>
+        <v>-16.809773544378125</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>18.645611851295953</v>
+        <v>-10.547508233445051</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>12.083907234213235</v>
+        <v>4.4739940168077439</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>28.281411240187936</v>
+        <v>15.341593684944463</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.368826011307519</v>
+        <v>11.920102873426849</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.192723317316197</v>
+        <v>-19.289965312715641</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0385609819049648</v>
+        <v>6.9119905708045657</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0077261474913186</v>
+        <v>-11.724289420315131</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>14.947030619064471</v>
+        <v>3.1871216485906153</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.926700919767669</v>
+        <v>5.8353437701364754</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.114326109754078</v>
+        <v>5.9438117862014863</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>15.055061820869646</v>
+        <v>15.380098459332153</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>18.571518179094575</v>
+        <v>6.4265576172393608</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.4065294312094085</v>
+        <v>-6.9643901699186923</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>18.647053319862003</v>
+        <v>13.908869467823862</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.135058007839067</v>
+        <v>25.827168103290504</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>17.988732583599585</v>
+        <v>-15.54524956803076</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>19.333456608541375</v>
+        <v>9.5934667707729702</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7293026569405647</v>
+        <v>6.9223672367539741</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.58533818405261329</v>
+        <v>22.570174025818567</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>27.467324493926959</v>
+        <v>19.014189262986925</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.283474299935321</v>
+        <v>23.1096976792726</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.123599123372887</v>
+        <v>-9.2168023542812048</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.197218232143566</v>
+        <v>13.209416867846066</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>18.808924988505659</v>
+        <v>8.2541019571614385</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9963143585461438</v>
+        <v>7.624379030047681</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>27.914658812138235</v>
+        <v>-18.668500643859485</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>15.672156057369989</v>
+        <v>3.0933369820161438</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.5299591243496167</v>
+        <v>-4.9712462003207776</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.951340346735595</v>
+        <v>23.386833537637429</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.513604336077151</v>
+        <v>6.5917819755282459</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.310095999019907</v>
+        <v>-18.205854038619485</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.325235080288266</v>
+        <v>-14.551341066317136</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8248238863869979</v>
+        <v>24.810854574142958</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.2641261551989516</v>
+        <v>5.4575841677263206</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.7266402786862987</v>
+        <v>17.066621861928148</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5725039343302427</v>
+        <v>8.6731184756294155</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.96474629048755</v>
+        <v>15.766317693833614</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>11.849305847560306</v>
+        <v>-1.876196758579372</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41455675902287936</v>
+        <v>22.405788312060807</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6405048951596832</v>
+        <v>2.9193632147592936</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.9335893453949264</v>
+        <v>10.937733052298867</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.695118274944981</v>
+        <v>15.934531430038668</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.890949101002558</v>
+        <v>-17.345161615672858</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.478162990221124</v>
+        <v>23.549830208237253</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.0540014508854494</v>
+        <v>-6.3582015450901128</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.12600969468782</v>
+        <v>14.677738698730145</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.4606539968355428</v>
+        <v>22.081381692889586</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>14.618334074582499</v>
+        <v>23.768196972558073</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>23.873849992891891</v>
+        <v>26.448605208096197</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.600871286120167</v>
+        <v>-11.852402975076147</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>27.974397202587724</v>
+        <v>8.2052775525647377</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2372246278463521</v>
+        <v>-16.277011496721716</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.379312925465079</v>
+        <v>-18.710051185388636</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0437667475302614</v>
+        <v>25.0067954887366</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.693675778564625</v>
+        <v>-15.532178414432106</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.029528767841875</v>
+        <v>24.647836891116285</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>26.153674653556379</v>
+        <v>8.055305395876001</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>21.079733413428094</v>
+        <v>5.4127459342985205</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.0095998503501118</v>
+        <v>-19.763856449800336</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3355121236044507</v>
+        <v>10.438594829493436</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1015973013243858</v>
+        <v>-9.2908871399391959</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>13.644642350494316</v>
+        <v>17.494442358889067</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.3881062140973555</v>
+        <v>17.974917707472414</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8139779138145045</v>
+        <v>-15.867895354277477</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8791673877206243</v>
+        <v>-2.2759294085415256</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>16.630333006103676</v>
+        <v>6.6111717639364826</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0950325318725334</v>
+        <v>-2.2772288996973309</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.75748966313343</v>
+        <v>13.114205494160984</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.65120416636535</v>
+        <v>5.4781302835673635</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.610784239656695</v>
+        <v>10.624849705843786</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.5496170053688303</v>
+        <v>14.631055006931746</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>26.865892395607823</v>
+        <v>-8.5181915646167319</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.810371930053627</v>
+        <v>29.159579174942429</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>17.505280023666103</v>
+        <v>-6.8497382888083376</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.367331415030506</v>
+        <v>-3.6823011120641489</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9849542559746851</v>
+        <v>18.223519505575723</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.128733105961235</v>
+        <v>28.364803172244443</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>28.224318423536815</v>
+        <v>26.65571213849389</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>11.015277407300189</v>
+        <v>-9.6546673613682952</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>28.445218306677496</v>
+        <v>6.5440415133640357</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7001169093597213</v>
+        <v>20.279808959877727</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.544683622285302</v>
+        <v>-4.3239463744322357</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7386164756081079</v>
+        <v>21.298355344634345</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>22.379365805984634</v>
+        <v>6.0136204997808385</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6763834755061424</v>
+        <v>-2.3328272474801715</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.842676717929088</v>
+        <v>-2.690302486808914</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>15.630519104404982</v>
+        <v>-6.7205425122915212</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.099716255163337</v>
+        <v>26.529183736975078</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.680716954628808</v>
+        <v>-4.0204644051968046</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>23.856329128263859</v>
+        <v>24.923073166181801</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60333251046352743</v>
+        <v>-6.6402032252471201</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>11.200646561724909</v>
+        <v>15.392904926706144</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>15.612587840893625</v>
+        <v>-8.4850556456893305</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.092343615995066</v>
+        <v>3.4692117911837599</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.56180106903733</v>
+        <v>21.49699431637633</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>22.242963242521107</v>
+        <v>-14.555594667831745</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.963982362511288</v>
+        <v>19.419090901349392</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>17.531008010933078</v>
+        <v>-18.462801863244366</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>25.798736415296787</v>
+        <v>3.718444047304942</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96884623021373528</v>
+        <v>-17.82540640242317</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>26.59969556735841</v>
+        <v>-17.017934370557263</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9563669619487456</v>
+        <v>-11.604455609963203</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.079926769389786</v>
+        <v>21.493441451246866</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>19.759333575808583</v>
+        <v>26.719531713732252</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.924596075261174</v>
+        <v>-3.261524753301984</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>10.497966871810167</v>
+        <v>-11.73441382436539</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.6724325831061169</v>
+        <v>-1.9672963485146511</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8947843663323241</v>
+        <v>-7.4035563661007711</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3448451028334816</v>
+        <v>-4.9027493648621672</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.059606444632244</v>
+        <v>-17.797845020379359</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.352750476524108</v>
+        <v>23.220656864590225</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9850168961287267</v>
+        <v>-7.7382646515708746</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>20.310386950835195</v>
+        <v>24.478525503213085</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>12.886933769815904</v>
+        <v>22.165485848989633</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.934806367993648</v>
+        <v>23.574898775637998</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.343532058659482</v>
+        <v>3.4575957488108102</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.249971346351991</v>
+        <v>6.436716397768933</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.196205413015884</v>
+        <v>19.043906138059107</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>27.858454695388296</v>
+        <v>13.977907696234688</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8780635172220954</v>
+        <v>20.583119506124433</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.229639497126509</v>
+        <v>18.89599455305742</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.75896143542556516</v>
+        <v>23.095652734425812</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0453222388175085</v>
+        <v>-2.9208859853989075</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.9209897569472965</v>
+        <v>28.03610211702231</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5853989166645448</v>
+        <v>-18.055874239335044</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7249190954489357</v>
+        <v>12.947735710944528</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52809539386344539</v>
+        <v>15.309604567070146</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4124339877836647</v>
+        <v>11.169401333520526</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.981748950548578</v>
+        <v>20.426584313205502</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.911718530389361</v>
+        <v>12.729831216587527</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8550504737141402</v>
+        <v>-15.764367475192675</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4576213702591438</v>
+        <v>-14.283415772912482</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>26.953432991967048</v>
+        <v>17.559016126614104</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>21.150104483274134</v>
+        <v>16.925543562776205</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.208178078612441</v>
+        <v>6.6140802565369867</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4916440511719244</v>
+        <v>26.366816287205921</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.743503942691362</v>
+        <v>27.047059415413919</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.466925660637038</v>
+        <v>-1.1179426973361579</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>27.276671857799329</v>
+        <v>-3.2883701612975926</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.070416285223576</v>
+        <v>-17.293773998751981</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4443263596795255</v>
+        <v>-13.470161935686065</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>27.100226500129622</v>
+        <v>3.96023845915024</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.542120939452222</v>
+        <v>12.660278478860384</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>20.552966267106271</v>
+        <v>-2.551600898152028</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7668341813527348</v>
+        <v>-2.3842411022048822</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.496066029006546</v>
+        <v>-17.55584966341193</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.162428919151601</v>
+        <v>-19.791235990228387</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.694202449859404</v>
+        <v>28.320866355329287</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>17.76591880160634</v>
+        <v>-4.3804347491015516</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>18.65924135887542</v>
+        <v>-1.5596061435717488</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>19.439177316838467</v>
+        <v>18.096364899366655</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7836500159640352</v>
+        <v>-11.694468363819482</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8950781826762011</v>
+        <v>9.8123846823164129</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>16.153342560394051</v>
+        <v>-17.433371781454532</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1801327877444763</v>
+        <v>-5.8675663101277244</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.422137248730962</v>
+        <v>5.3025211916908468</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.029852260672477</v>
+        <v>6.8935289792324959</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>28.374839014687446</v>
+        <v>-4.5182370871452093</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>14.318859899433313</v>
+        <v>-16.821080440193864</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9550407594913608</v>
+        <v>27.274749090385157</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>27.851196048038133</v>
+        <v>-15.385419314215092</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1463196958436548</v>
+        <v>29.5689104817776</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.2929788774371271</v>
+        <v>12.999667751988895</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62692690789705452</v>
+        <v>4.466009985919861</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2838259859460983</v>
+        <v>7.7172889067099817</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9307680490612462</v>
+        <v>1.458529319569962</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2954379064418475</v>
+        <v>-8.4864744334753546</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>20.401712941253322</v>
+        <v>-16.995350566311139</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.602307370217673</v>
+        <v>15.298067596092537</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.206841020195256</v>
+        <v>20.326314176478299</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3244986998535069</v>
+        <v>-2.7548135664315296</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.452511658490572</v>
+        <v>27.165517142157043</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>13.878159341328271</v>
+        <v>-17.680667096773632</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>24.360452354693891</v>
+        <v>17.462574098155407</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>16.746569913242048</v>
+        <v>1.8927526307074629</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>16.833242827273303</v>
+        <v>3.8011575905372759</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>24.04623007466062</v>
+        <v>18.391247469748372</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.746104954743668</v>
+        <v>8.8376341443842037</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>25.493911283833761</v>
+        <v>-14.100752897312223</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1738553361260635</v>
+        <v>-14.742738107924858</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>14.531341353781499</v>
+        <v>24.103589043590944</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.337173854851937</v>
+        <v>-13.065981446860597</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.607358694934742</v>
+        <v>-4.4035901383797409</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7297539945930716</v>
+        <v>-8.3420798572378878</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4988896007168577</v>
+        <v>-14.49331715498267</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9085584334929671</v>
+        <v>28.538314155881068</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.549378417754077</v>
+        <v>-8.5641204917242462</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7689551564853794</v>
+        <v>-16.804450585224767</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4780799638945084</v>
+        <v>26.292411071135483</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.1036300471121194</v>
+        <v>-17.824551492440513</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.3649087110506297</v>
+        <v>21.343018776739065</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.641300316660196</v>
+        <v>-6.7906653546349993</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9712044636718105</v>
+        <v>25.177596531639068</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>21.440954040055111</v>
+        <v>19.833412020723166</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.885069650369157</v>
+        <v>-6.6460830072458617</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>12.937920969693003</v>
+        <v>9.1663120119582224</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.239165742862362</v>
+        <v>-12.109558397413121</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.651596692669923</v>
+        <v>22.670580278478447</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>21.974382660582116</v>
+        <v>1.1312802852010151</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.6139542470220558</v>
+        <v>24.958274123196823</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>17.43646017685986</v>
+        <v>-11.061029645608793</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>13.981209225914306</v>
+        <v>10.018667513521557</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.580840502407218</v>
+        <v>7.0886842871211293</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.95239238139505</v>
+        <v>-16.802835804956029</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>26.872318810015393</v>
+        <v>23.322027429368745</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.809830872406232</v>
+        <v>-12.68455730453104</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.599696276250178</v>
+        <v>-3.8246759690527625</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0953218062926666</v>
+        <v>12.242453446978949</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9342633290650681</v>
+        <v>-17.960048377441645</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>14.750464782200844</v>
+        <v>-17.422177886299536</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>15.806833133794349</v>
+        <v>26.071144762207418</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>18.963449887835537</v>
+        <v>-1.2032986604077145</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.85096645207777044</v>
+        <v>14.465180929406131</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>18.183783081185247</v>
+        <v>16.364571809156061</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.81563033161479126</v>
+        <v>11.757042189460062</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1491462749084356</v>
+        <v>15.750026759631595</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>12.151746246359465</v>
+        <v>-0.90268433951919391</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89925261933894163</v>
+        <v>2.5571252425145374</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2104573366327891</v>
+        <v>-17.883746179837331</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>27.911985142018281</v>
+        <v>-10.366515254508512</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>27.629776933320201</v>
+        <v>2.4188535080181452</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>12.068313492496763</v>
+        <v>23.107151524509227</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18637285220194855</v>
+        <v>-12.804393983930572</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.64282608199730973</v>
+        <v>2.0235111132314572</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>18.155971315111579</v>
+        <v>10.30685288403539</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5428349536941468</v>
+        <v>3.8398001877418828</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.374492637491349</v>
+        <v>-1.6317644880525286</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.827251271917785</v>
+        <v>12.611375269362476</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>22.930734909577268</v>
+        <v>1.2813562953972735E-3</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>23.4760453681684</v>
+        <v>26.414476027553761</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.4663185532244647</v>
+        <v>-19.861756142632572</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.652932437630234</v>
+        <v>15.507723896068647</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.881229517033582</v>
+        <v>-11.723622471081152</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.606584868699359</v>
+        <v>-2.6223460079767165</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.64802343859462</v>
+        <v>-10.460937909839018</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27381590646270126</v>
+        <v>25.306432284162625</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>11.251982780144687</v>
+        <v>-17.834713040379036</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>23.513646328702208</v>
+        <v>-17.636002727696685</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.4063741323833341</v>
+        <v>27.124866123927561</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0410616648240811</v>
+        <v>28.212017171155615</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>17.002890520180792</v>
+        <v>-15.08185233348836</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.266973713910009</v>
+        <v>24.730873521777056</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>15.995015486181813</v>
+        <v>-14.625412713666224</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3728382494831894</v>
+        <v>13.130988625267733</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>19.212754081964341</v>
+        <v>-14.115028920533616</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2318799068850179</v>
+        <v>6.6989401893146585</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>20.493550703881603</v>
+        <v>4.146676996694648</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.028296432342273</v>
+        <v>27.219525888821238</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>18.055931539008569</v>
+        <v>11.44910248588544</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.437009029296361</v>
+        <v>16.396316040931772</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>15.34142699614231</v>
+        <v>25.115293217796946</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.67802318241493609</v>
+        <v>8.1843953449463882</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>18.110068544688467</v>
+        <v>6.8557386601197052</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.13930217806739975</v>
+        <v>15.81967524607704</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3706731249594633</v>
+        <v>-4.7219829658831962</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>28.261086266013933</v>
+        <v>19.445158006936296</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.633686213494268</v>
+        <v>3.0096621047416292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>